<commit_message>
[note]: obsah a reserse vysledkove casti
</commit_message>
<xml_diff>
--- a/bc - tabulka výsledky.xlsx
+++ b/bc - tabulka výsledky.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7275a55917014348/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7275a55917014348/Desktop/bakalarka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1317" documentId="8_{BE3E68FC-0BCD-49A6-9D79-EB778FD7412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B6DD12B-C9CF-4A0B-9B63-323FBB533B80}"/>
+  <xr:revisionPtr revIDLastSave="1407" documentId="8_{BE3E68FC-0BCD-49A6-9D79-EB778FD7412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{707C0FB7-5861-4BE0-8C2F-4C6CE5C06F4A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EC50F4EA-C447-47CC-B6F2-DF478986B29A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19230" windowHeight="21000" xr2:uid="{EC50F4EA-C447-47CC-B6F2-DF478986B29A}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1638,9 +1638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B613202B-7148-46E5-915C-6F5F12744654}">
   <dimension ref="A1:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="88" zoomScaleNormal="25" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="25" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
[note]: vertical jumps a uvod
</commit_message>
<xml_diff>
--- a/bc - tabulka výsledky.xlsx
+++ b/bc - tabulka výsledky.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7275a55917014348/Desktop/bakalarka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1407" documentId="8_{BE3E68FC-0BCD-49A6-9D79-EB778FD7412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{707C0FB7-5861-4BE0-8C2F-4C6CE5C06F4A}"/>
+  <xr:revisionPtr revIDLastSave="1412" documentId="8_{BE3E68FC-0BCD-49A6-9D79-EB778FD7412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6C0231A-9D3A-4E4C-8425-4A207B18230D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19230" windowHeight="21000" xr2:uid="{EC50F4EA-C447-47CC-B6F2-DF478986B29A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10740" xr2:uid="{EC50F4EA-C447-47CC-B6F2-DF478986B29A}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1638,9 +1638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B613202B-7148-46E5-915C-6F5F12744654}">
   <dimension ref="A1:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="25" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2198,219 +2198,215 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>16</v>
+        <v>153</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>53</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="C10" s="13"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="K10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="15" t="s">
+        <v>168</v>
+      </c>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
+      <c r="N10" s="15" t="s">
+        <v>259</v>
+      </c>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
-      <c r="Q10" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="R10" s="15" t="s">
-        <v>235</v>
-      </c>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
-      <c r="W10" s="15" t="s">
-        <v>312</v>
-      </c>
+      <c r="W10" s="13"/>
       <c r="X10" s="13"/>
-      <c r="Y10" s="15" t="s">
-        <v>313</v>
-      </c>
+      <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
-      <c r="AA10" s="15" t="s">
-        <v>314</v>
-      </c>
+      <c r="AA10" s="13"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>54</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="E11" s="2" t="s">
-        <v>72</v>
+      <c r="E11" s="15" t="s">
+        <v>96</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>117</v>
+        <v>103</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>237</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R11" s="15" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
       <c r="U11" s="13"/>
-      <c r="V11" s="2" t="s">
-        <v>315</v>
-      </c>
+      <c r="V11" s="13"/>
       <c r="W11" s="15" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="15" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="Z11" s="13"/>
       <c r="AA11" s="15" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="D12" s="13"/>
-      <c r="E12" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="13"/>
+      <c r="E12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="G12" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="H12" s="13"/>
+        <v>104</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="I12" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
+        <v>144</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>237</v>
+      </c>
       <c r="O12" s="13"/>
-      <c r="P12" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>238</v>
+      </c>
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
+      <c r="V12" s="2" t="s">
+        <v>315</v>
+      </c>
       <c r="W12" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="X12" s="13"/>
-      <c r="Y12" s="13"/>
+      <c r="Y12" s="15" t="s">
+        <v>317</v>
+      </c>
       <c r="Z12" s="13"/>
       <c r="AA12" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>279</v>
+        <v>13</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="G13" s="15" t="s">
+        <v>105</v>
+      </c>
       <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="I13" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>145</v>
+      </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
+      <c r="P13" s="15" t="s">
+        <v>180</v>
+      </c>
       <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
       <c r="S13" s="13"/>
-      <c r="T13" s="15" t="s">
-        <v>274</v>
-      </c>
+      <c r="T13" s="13"/>
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
+      <c r="W13" s="15" t="s">
+        <v>319</v>
+      </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
-      <c r="Z13" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="AA13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="15" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="B14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="7"/>
+        <v>279</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="15" t="s">
-        <v>106</v>
-      </c>
+      <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
@@ -2418,123 +2414,130 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
-      <c r="O14" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="P14" s="15" t="s">
-        <v>179</v>
-      </c>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
-      <c r="S14" s="15" t="s">
+      <c r="S14" s="13"/>
+      <c r="T14" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="AA14" s="13"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="P15" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="T14" s="13"/>
-      <c r="U14" s="15" t="s">
+      <c r="T15" s="13"/>
+      <c r="U15" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="V14" s="15" t="s">
+      <c r="V15" s="15" t="s">
         <v>283</v>
       </c>
-      <c r="W14" s="15" t="s">
+      <c r="W15" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="X14" s="15" t="s">
+      <c r="X15" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="B15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="L15" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="M15" s="13"/>
-      <c r="N15" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
       <c r="Z15" s="13"/>
       <c r="AA15" s="13"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
-        <v>275</v>
+        <v>10</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="15" t="s">
+        <v>74</v>
+      </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
+      <c r="H16" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>134</v>
+      </c>
       <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+      <c r="K16" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>240</v>
+      </c>
       <c r="M16" s="13"/>
-      <c r="N16" s="21"/>
+      <c r="N16" s="19" t="s">
+        <v>241</v>
+      </c>
       <c r="O16" s="13"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
+      <c r="R16" s="15" t="s">
+        <v>242</v>
+      </c>
       <c r="S16" s="13"/>
-      <c r="T16" s="15" t="s">
-        <v>323</v>
-      </c>
+      <c r="T16" s="13"/>
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
       <c r="W16" s="13"/>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
-      <c r="Z16" s="15" t="s">
-        <v>324</v>
-      </c>
+      <c r="Z16" s="13"/>
       <c r="AA16" s="13"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="11"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
-      <c r="I17" s="11"/>
+      <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -2546,7 +2549,7 @@
       <c r="R17" s="13"/>
       <c r="S17" s="13"/>
       <c r="T17" s="15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="U17" s="13"/>
       <c r="V17" s="13"/>
@@ -2554,24 +2557,21 @@
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
       <c r="Z17" s="15" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AA17" s="13"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>277</v>
-      </c>
       <c r="B18" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
+      <c r="E18" s="11"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
+      <c r="I18" s="11"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
@@ -2583,7 +2583,7 @@
       <c r="R18" s="13"/>
       <c r="S18" s="13"/>
       <c r="T18" s="15" t="s">
-        <v>280</v>
+        <v>325</v>
       </c>
       <c r="U18" s="13"/>
       <c r="V18" s="13"/>
@@ -2591,64 +2591,65 @@
       <c r="X18" s="13"/>
       <c r="Y18" s="13"/>
       <c r="Z18" s="15" t="s">
-        <v>297</v>
+        <v>326</v>
       </c>
       <c r="AA18" s="13"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>9</v>
+        <v>277</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>55</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="C19" s="13"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="17"/>
+      <c r="I19" s="13"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
+      <c r="N19" s="21"/>
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="15" t="s">
-        <v>243</v>
-      </c>
+      <c r="R19" s="13"/>
       <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
+      <c r="T19" s="15" t="s">
+        <v>280</v>
+      </c>
       <c r="U19" s="13"/>
       <c r="V19" s="13"/>
       <c r="W19" s="13"/>
       <c r="X19" s="13"/>
       <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
+      <c r="Z19" s="15" t="s">
+        <v>297</v>
+      </c>
       <c r="AA19" s="13"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="B20" s="6" t="s">
-        <v>271</v>
+        <v>8</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="15" t="s">
-        <v>76</v>
+      <c r="E20" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="I20" s="17"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
@@ -2658,7 +2659,7 @@
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>
       <c r="R20" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="S20" s="13"/>
       <c r="T20" s="13"/>
@@ -2672,14 +2673,14 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>57</v>
+        <v>271</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="D21" s="13"/>
-      <c r="E21" s="2" t="s">
-        <v>77</v>
+      <c r="E21" s="15" t="s">
+        <v>76</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -2694,7 +2695,7 @@
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
       <c r="R21" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="S21" s="13"/>
       <c r="T21" s="13"/>
@@ -2706,123 +2707,123 @@
       <c r="Z21" s="13"/>
       <c r="AA21" s="13"/>
     </row>
-    <row r="22" spans="1:27" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="6" t="s">
-        <v>6</v>
-      </c>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>58</v>
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="D22" s="13"/>
-      <c r="E22" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>119</v>
-      </c>
+      <c r="E22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
       <c r="I22" s="13"/>
-      <c r="J22" s="15" t="s">
-        <v>146</v>
-      </c>
+      <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
       <c r="N22" s="13"/>
-      <c r="O22" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="P22" s="15" t="s">
-        <v>269</v>
-      </c>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="15" t="s">
-        <v>272</v>
-      </c>
+      <c r="R22" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="S22" s="13"/>
       <c r="T22" s="13"/>
-      <c r="U22" s="15" t="s">
-        <v>327</v>
-      </c>
+      <c r="U22" s="13"/>
       <c r="V22" s="13"/>
-      <c r="W22" s="15" t="s">
-        <v>328</v>
-      </c>
-      <c r="X22" s="15" t="s">
-        <v>294</v>
-      </c>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
       <c r="Y22" s="13"/>
       <c r="Z22" s="13"/>
       <c r="AA22" s="13"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="B23" s="6" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>62</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D23" s="13"/>
       <c r="E23" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+        <v>78</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>110</v>
+      </c>
       <c r="H23" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
+      <c r="J23" s="15" t="s">
+        <v>146</v>
+      </c>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
+      <c r="O23" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="P23" s="15" t="s">
+        <v>269</v>
+      </c>
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
+      <c r="S23" s="15" t="s">
+        <v>272</v>
+      </c>
       <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
+      <c r="U23" s="15" t="s">
+        <v>327</v>
+      </c>
       <c r="V23" s="13"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="13"/>
+      <c r="W23" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="X23" s="15" t="s">
+        <v>294</v>
+      </c>
       <c r="Y23" s="13"/>
       <c r="Z23" s="13"/>
       <c r="AA23" s="13"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="22" t="s">
-        <v>218</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="13"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="H24" s="15" t="s">
+        <v>120</v>
+      </c>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
-      <c r="K24" s="22" t="s">
-        <v>219</v>
-      </c>
+      <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
-      <c r="N24" s="23" t="s">
-        <v>267</v>
-      </c>
+      <c r="N24" s="13"/>
       <c r="O24" s="13"/>
       <c r="P24" s="13"/>
       <c r="Q24" s="13"/>
@@ -2838,54 +2839,52 @@
       <c r="AA24" s="13"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="B25" s="6" t="s">
-        <v>172</v>
+        <v>217</v>
       </c>
       <c r="C25" s="11"/>
-      <c r="D25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="22" t="s">
+        <v>218</v>
+      </c>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
+      <c r="K25" s="22" t="s">
+        <v>219</v>
+      </c>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="P25" s="15" t="s">
-        <v>183</v>
-      </c>
+      <c r="N25" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
-      <c r="S25" s="15" t="s">
-        <v>206</v>
-      </c>
+      <c r="S25" s="13"/>
       <c r="T25" s="13"/>
       <c r="U25" s="13"/>
       <c r="V25" s="13"/>
       <c r="W25" s="13"/>
-      <c r="X25" s="15" t="s">
-        <v>292</v>
-      </c>
+      <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
       <c r="Z25" s="13"/>
       <c r="AA25" s="13"/>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="B26" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C26" s="11"/>
-      <c r="D26" s="13"/>
+      <c r="D26" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -2894,27 +2893,33 @@
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
-      <c r="M26" s="15" t="s">
-        <v>177</v>
-      </c>
+      <c r="M26" s="13"/>
       <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
+      <c r="O26" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="P26" s="15" t="s">
+        <v>183</v>
+      </c>
       <c r="Q26" s="13"/>
       <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
+      <c r="S26" s="15" t="s">
+        <v>206</v>
+      </c>
       <c r="T26" s="13"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
       <c r="W26" s="13"/>
-      <c r="X26" s="13"/>
+      <c r="X26" s="15" t="s">
+        <v>292</v>
+      </c>
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
       <c r="AA26" s="13"/>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="13"/>
@@ -2927,13 +2932,11 @@
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
-      <c r="P27" s="15" t="s">
-        <v>182</v>
-      </c>
+      <c r="P27" s="13"/>
       <c r="Q27" s="13"/>
       <c r="R27" s="13"/>
       <c r="S27" s="13"/>
@@ -2947,112 +2950,112 @@
       <c r="AA27" s="13"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>213</v>
-      </c>
       <c r="B28" s="6" t="s">
-        <v>211</v>
+        <v>171</v>
       </c>
       <c r="C28" s="11"/>
-      <c r="D28" s="15" t="s">
-        <v>64</v>
-      </c>
+      <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
-      <c r="G28" s="15" t="s">
-        <v>107</v>
-      </c>
+      <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
-      <c r="K28" s="15" t="s">
-        <v>163</v>
-      </c>
+      <c r="K28" s="13"/>
       <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="O28" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="P28" s="13"/>
+      <c r="M28" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="15" t="s">
+        <v>182</v>
+      </c>
       <c r="Q28" s="13"/>
       <c r="R28" s="13"/>
-      <c r="S28" s="15" t="s">
-        <v>207</v>
-      </c>
+      <c r="S28" s="13"/>
       <c r="T28" s="13"/>
-      <c r="U28" s="22" t="s">
-        <v>329</v>
-      </c>
-      <c r="V28" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="W28" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="X28" s="15" t="s">
-        <v>291</v>
-      </c>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
       <c r="Z28" s="13"/>
-      <c r="AA28" s="15" t="s">
-        <v>332</v>
-      </c>
+      <c r="AA28" s="13"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>213</v>
+      </c>
       <c r="B29" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C29" s="11"/>
-      <c r="D29" s="13"/>
+      <c r="D29" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="22" t="s">
-        <v>121</v>
-      </c>
+      <c r="G29" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="H29" s="13"/>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
+      <c r="K29" s="15" t="s">
+        <v>163</v>
+      </c>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="13"/>
+      <c r="N29" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="O29" s="15" t="s">
+        <v>249</v>
+      </c>
       <c r="P29" s="13"/>
       <c r="Q29" s="13"/>
       <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
+      <c r="S29" s="15" t="s">
+        <v>207</v>
+      </c>
       <c r="T29" s="13"/>
-      <c r="U29" s="13"/>
-      <c r="V29" s="13"/>
-      <c r="W29" s="13"/>
-      <c r="X29" s="13"/>
+      <c r="U29" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="V29" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="W29" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="X29" s="15" t="s">
+        <v>291</v>
+      </c>
       <c r="Y29" s="13"/>
       <c r="Z29" s="13"/>
-      <c r="AA29" s="13"/>
+      <c r="AA29" s="15" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="13"/>
-      <c r="E30" s="7"/>
+      <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="H30" s="22" t="s">
+        <v>121</v>
+      </c>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
-      <c r="K30" s="18" t="s">
-        <v>250</v>
-      </c>
+      <c r="K30" s="13"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
-      <c r="N30" s="19" t="s">
-        <v>251</v>
-      </c>
+      <c r="N30" s="21"/>
       <c r="O30" s="13"/>
       <c r="P30" s="13"/>
       <c r="Q30" s="13"/>
@@ -3060,9 +3063,7 @@
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
       <c r="U30" s="13"/>
-      <c r="V30" s="15" t="s">
-        <v>333</v>
-      </c>
+      <c r="V30" s="13"/>
       <c r="W30" s="13"/>
       <c r="X30" s="13"/>
       <c r="Y30" s="13"/>
@@ -3070,26 +3071,25 @@
       <c r="AA30" s="13"/>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>111</v>
-      </c>
       <c r="B31" s="6" t="s">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="15" t="s">
-        <v>94</v>
-      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
+      <c r="K31" s="18" t="s">
+        <v>250</v>
+      </c>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
+      <c r="N31" s="19" t="s">
+        <v>251</v>
+      </c>
       <c r="O31" s="13"/>
       <c r="P31" s="13"/>
       <c r="Q31" s="13"/>
@@ -3097,7 +3097,9 @@
       <c r="S31" s="13"/>
       <c r="T31" s="13"/>
       <c r="U31" s="13"/>
-      <c r="V31" s="13"/>
+      <c r="V31" s="15" t="s">
+        <v>333</v>
+      </c>
       <c r="W31" s="13"/>
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
@@ -3105,29 +3107,28 @@
       <c r="AA31" s="13"/>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="B32" s="6" t="s">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="F32" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="G32" s="13"/>
-      <c r="H32" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>135</v>
-      </c>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
       <c r="O32" s="13"/>
-      <c r="P32" s="15" t="s">
-        <v>181</v>
-      </c>
+      <c r="P32" s="13"/>
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
       <c r="S32" s="13"/>
@@ -3141,57 +3142,47 @@
       <c r="AA32" s="13"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>100</v>
-      </c>
       <c r="B33" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="13"/>
+        <v>112</v>
+      </c>
+      <c r="C33" s="11"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
-      <c r="G33" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="H33" s="13"/>
-      <c r="I33" s="22" t="s">
-        <v>342</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="K33" s="15" t="s">
-        <v>164</v>
-      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
       <c r="L33" s="13"/>
       <c r="M33" s="13"/>
-      <c r="N33" s="15" t="s">
-        <v>252</v>
-      </c>
+      <c r="N33" s="13"/>
       <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
+      <c r="P33" s="15" t="s">
+        <v>181</v>
+      </c>
       <c r="Q33" s="13"/>
       <c r="R33" s="13"/>
       <c r="S33" s="13"/>
       <c r="T33" s="13"/>
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
-      <c r="W33" s="15" t="s">
-        <v>334</v>
-      </c>
-      <c r="X33" s="15" t="s">
-        <v>290</v>
-      </c>
+      <c r="W33" s="13"/>
+      <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
       <c r="Z33" s="13"/>
-      <c r="AA33" s="15" t="s">
-        <v>335</v>
-      </c>
+      <c r="AA33" s="13"/>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="B34" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -3202,10 +3193,10 @@
       </c>
       <c r="H34" s="13"/>
       <c r="I34" s="22" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K34" s="15" t="s">
         <v>164</v>
@@ -3213,7 +3204,7 @@
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
       <c r="N34" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
@@ -3236,29 +3227,30 @@
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="B35" s="6" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
+      <c r="I35" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>148</v>
+      </c>
       <c r="K35" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
-      <c r="N35" s="2" t="s">
-        <v>254</v>
+      <c r="N35" s="15" t="s">
+        <v>253</v>
       </c>
       <c r="O35" s="13"/>
       <c r="P35" s="13"/>
@@ -3267,43 +3259,43 @@
       <c r="S35" s="13"/>
       <c r="T35" s="13"/>
       <c r="U35" s="13"/>
-      <c r="V35" s="15" t="s">
-        <v>282</v>
-      </c>
+      <c r="V35" s="13"/>
       <c r="W35" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="X35" s="13"/>
+        <v>334</v>
+      </c>
+      <c r="X35" s="15" t="s">
+        <v>290</v>
+      </c>
       <c r="Y35" s="13"/>
       <c r="Z35" s="13"/>
-      <c r="AA35" s="13"/>
+      <c r="AA35" s="15" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="15" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
       <c r="K36" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="L36" s="15" t="s">
-        <v>255</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="L36" s="13"/>
       <c r="M36" s="13"/>
-      <c r="N36" s="19" t="s">
-        <v>256</v>
+      <c r="N36" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="O36" s="13"/>
       <c r="P36" s="13"/>
@@ -3313,10 +3305,10 @@
       <c r="T36" s="13"/>
       <c r="U36" s="13"/>
       <c r="V36" s="15" t="s">
-        <v>337</v>
+        <v>282</v>
       </c>
       <c r="W36" s="15" t="s">
-        <v>286</v>
+        <v>336</v>
       </c>
       <c r="X36" s="13"/>
       <c r="Y36" s="13"/>
@@ -3325,25 +3317,31 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>209</v>
+        <v>152</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>191</v>
+        <v>8</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="16" t="s">
-        <v>123</v>
-      </c>
+      <c r="G37" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H37" s="13"/>
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
+      <c r="K37" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="L37" s="15" t="s">
+        <v>255</v>
+      </c>
       <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
+      <c r="N37" s="19" t="s">
+        <v>256</v>
+      </c>
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
       <c r="Q37" s="13"/>
@@ -3351,23 +3349,32 @@
       <c r="S37" s="13"/>
       <c r="T37" s="13"/>
       <c r="U37" s="13"/>
-      <c r="V37" s="13"/>
-      <c r="W37" s="13"/>
+      <c r="V37" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="W37" s="15" t="s">
+        <v>286</v>
+      </c>
       <c r="X37" s="13"/>
       <c r="Y37" s="13"/>
       <c r="Z37" s="13"/>
       <c r="AA37" s="13"/>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
+        <v>209</v>
+      </c>
       <c r="B38" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="H38" s="16" t="s">
+        <v>123</v>
+      </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
@@ -3376,9 +3383,7 @@
       <c r="N38" s="13"/>
       <c r="O38" s="13"/>
       <c r="P38" s="13"/>
-      <c r="Q38" s="15" t="s">
-        <v>193</v>
-      </c>
+      <c r="Q38" s="13"/>
       <c r="R38" s="13"/>
       <c r="S38" s="13"/>
       <c r="T38" s="13"/>
@@ -3386,18 +3391,13 @@
       <c r="V38" s="13"/>
       <c r="W38" s="13"/>
       <c r="X38" s="13"/>
-      <c r="Y38" s="15" t="s">
-        <v>338</v>
-      </c>
+      <c r="Y38" s="13"/>
       <c r="Z38" s="13"/>
       <c r="AA38" s="13"/>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
-        <v>136</v>
-      </c>
       <c r="B39" s="6" t="s">
-        <v>137</v>
+        <v>192</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
@@ -3405,9 +3405,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="15" t="s">
-        <v>138</v>
-      </c>
+      <c r="I39" s="13"/>
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
@@ -3415,7 +3413,9 @@
       <c r="N39" s="13"/>
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
-      <c r="Q39" s="13"/>
+      <c r="Q39" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="R39" s="13"/>
       <c r="S39" s="13"/>
       <c r="T39" s="13"/>
@@ -3423,16 +3423,18 @@
       <c r="V39" s="13"/>
       <c r="W39" s="13"/>
       <c r="X39" s="13"/>
-      <c r="Y39" s="13"/>
+      <c r="Y39" s="15" t="s">
+        <v>338</v>
+      </c>
       <c r="Z39" s="13"/>
       <c r="AA39" s="13"/>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
@@ -3440,18 +3442,14 @@
       <c r="F40" s="13"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
+      <c r="I40" s="15" t="s">
+        <v>138</v>
+      </c>
       <c r="J40" s="13"/>
-      <c r="K40" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="L40" s="15" t="s">
-        <v>257</v>
-      </c>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
       <c r="M40" s="13"/>
-      <c r="N40" s="15" t="s">
-        <v>258</v>
-      </c>
+      <c r="N40" s="13"/>
       <c r="O40" s="13"/>
       <c r="P40" s="13"/>
       <c r="Q40" s="13"/>
@@ -3468,10 +3466,10 @@
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>155</v>
+        <v>17</v>
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
@@ -3482,12 +3480,14 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
       <c r="K41" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="L41" s="13"/>
+        <v>167</v>
+      </c>
+      <c r="L41" s="15" t="s">
+        <v>257</v>
+      </c>
       <c r="M41" s="13"/>
       <c r="N41" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O41" s="13"/>
       <c r="P41" s="13"/>

</xml_diff>

<commit_message>
[note]: tabulka, popis testu a jeste enco malo
</commit_message>
<xml_diff>
--- a/bc - tabulka výsledky.xlsx
+++ b/bc - tabulka výsledky.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7275a55917014348/Desktop/bakalarka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1489" documentId="8_{BE3E68FC-0BCD-49A6-9D79-EB778FD7412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67FA48DC-A3B0-4175-B939-4B491C7D0B01}"/>
+  <xr:revisionPtr revIDLastSave="1713" documentId="8_{BE3E68FC-0BCD-49A6-9D79-EB778FD7412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0759D99-FAB2-4D22-ADE1-F97F841E0502}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EC50F4EA-C447-47CC-B6F2-DF478986B29A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{EC50F4EA-C447-47CC-B6F2-DF478986B29A}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="TABULKA" sheetId="1" r:id="rId1"/>
+    <sheet name="List4" sheetId="4" r:id="rId2"/>
+    <sheet name="List2" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="351">
   <si>
     <t>⌀ vzdálenost přes hlavu (m)</t>
   </si>
@@ -1091,12 +1093,36 @@
   <si>
     <t>MAR (maximální aerobní rychlost) (km/h)</t>
   </si>
+  <si>
+    <t>15-15,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⌀ věk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">⌀ počet účastníků </t>
+  </si>
+  <si>
+    <t>Studie</t>
+  </si>
+  <si>
+    <t>úsek 10 metrů</t>
+  </si>
+  <si>
+    <t>úsek 30 metrů</t>
+  </si>
+  <si>
+    <t>Mé výsledky</t>
+  </si>
+  <si>
+    <t>Výsledky studií</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1119,6 +1145,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1153,7 +1185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1250,11 +1282,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1328,6 +1455,48 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -1648,22 +1817,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B613202B-7148-46E5-915C-6F5F12744654}">
   <dimension ref="A1:AA58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38:XFD40"/>
+      <selection pane="bottomRight" sqref="A1:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="36.21875" style="6" customWidth="1"/>
-    <col min="3" max="27" width="13.77734375" style="6" customWidth="1"/>
-    <col min="28" max="16384" width="9.21875" style="6"/>
+    <col min="1" max="1" width="31.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" style="6" customWidth="1"/>
+    <col min="3" max="27" width="13.7109375" style="6" customWidth="1"/>
+    <col min="28" max="16384" width="9.28515625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
@@ -1743,7 +1912,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>44</v>
       </c>
@@ -1823,7 +1992,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1903,7 +2072,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>101</v>
       </c>
@@ -1956,7 +2125,7 @@
       <c r="Z4" s="7"/>
       <c r="AA4" s="14"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
@@ -2008,7 +2177,7 @@
       <c r="Z5" s="13"/>
       <c r="AA5" s="11"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
@@ -2058,7 +2227,7 @@
       </c>
       <c r="AA6" s="11"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
@@ -2120,7 +2289,7 @@
       <c r="Z7" s="13"/>
       <c r="AA7" s="11"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>269</v>
       </c>
@@ -2167,7 +2336,7 @@
       <c r="Z8" s="13"/>
       <c r="AA8" s="13"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -2208,7 +2377,7 @@
       <c r="Z9" s="13"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>152</v>
       </c>
@@ -2245,7 +2414,7 @@
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
@@ -2302,7 +2471,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -2366,7 +2535,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
@@ -2410,7 +2579,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>277</v>
       </c>
@@ -2444,7 +2613,7 @@
       </c>
       <c r="AA14" s="13"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
@@ -2495,7 +2664,7 @@
       <c r="Z15" s="13"/>
       <c r="AA15" s="13"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2539,7 +2708,7 @@
       <c r="Z16" s="13"/>
       <c r="AA16" s="13"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>273</v>
       </c>
@@ -2573,7 +2742,7 @@
       </c>
       <c r="AA17" s="13"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>274</v>
       </c>
@@ -2607,7 +2776,7 @@
       </c>
       <c r="AA18" s="13"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>275</v>
       </c>
@@ -2644,7 +2813,7 @@
       </c>
       <c r="AA19" s="13"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
@@ -2687,7 +2856,7 @@
       <c r="Z20" s="13"/>
       <c r="AA20" s="13"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>172</v>
       </c>
@@ -2719,7 +2888,7 @@
       <c r="Z21" s="13"/>
       <c r="AA21" s="13"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>170</v>
       </c>
@@ -2753,7 +2922,7 @@
       <c r="Z22" s="13"/>
       <c r="AA22" s="13"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>110</v>
       </c>
@@ -2788,7 +2957,7 @@
       <c r="Z23" s="13"/>
       <c r="AA23" s="13"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>111</v>
       </c>
@@ -2824,7 +2993,7 @@
       <c r="Z24" s="13"/>
       <c r="AA24" s="13"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>99</v>
       </c>
@@ -2873,7 +3042,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>97</v>
       </c>
@@ -2919,7 +3088,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>188</v>
       </c>
@@ -2956,7 +3125,7 @@
       <c r="Z27" s="13"/>
       <c r="AA27" s="13"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>189</v>
       </c>
@@ -2993,7 +3162,7 @@
       <c r="Z28" s="13"/>
       <c r="AA28" s="13"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>135</v>
       </c>
@@ -3028,7 +3197,7 @@
       <c r="Z29" s="13"/>
       <c r="AA29" s="13"/>
     </row>
-    <row r="30" spans="1:27" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>341</v>
       </c>
@@ -3085,7 +3254,7 @@
       <c r="Z30" s="13"/>
       <c r="AA30" s="13"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>342</v>
       </c>
@@ -3123,13 +3292,13 @@
       <c r="Z31" s="13"/>
       <c r="AA31" s="13"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>216</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="13"/>
-      <c r="E32" s="7"/>
+      <c r="E32" s="13"/>
       <c r="F32" s="21" t="s">
         <v>217</v>
       </c>
@@ -3159,7 +3328,7 @@
       <c r="Z32" s="13"/>
       <c r="AA32" s="13"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>8</v>
       </c>
@@ -3198,7 +3367,7 @@
       <c r="Z33" s="13"/>
       <c r="AA33" s="13"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>270</v>
       </c>
@@ -3234,7 +3403,7 @@
       <c r="Z34" s="13"/>
       <c r="AA34" s="13"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>6</v>
       </c>
@@ -3270,7 +3439,7 @@
       <c r="Z35" s="13"/>
       <c r="AA35" s="13"/>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>151</v>
       </c>
@@ -3315,7 +3484,7 @@
       <c r="Z36" s="13"/>
       <c r="AA36" s="13"/>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>98</v>
       </c>
@@ -3358,7 +3527,7 @@
       <c r="Z37" s="13"/>
       <c r="AA37" s="13"/>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>212</v>
       </c>
@@ -3413,7 +3582,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>211</v>
       </c>
@@ -3445,7 +3614,7 @@
       <c r="Z39" s="13"/>
       <c r="AA39" s="13"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>209</v>
       </c>
@@ -3481,7 +3650,7 @@
       <c r="Z40" s="13"/>
       <c r="AA40" s="13"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>150</v>
       </c>
@@ -3520,7 +3689,7 @@
       <c r="Z41" s="13"/>
       <c r="AA41" s="13"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>153</v>
       </c>
@@ -3559,7 +3728,7 @@
       <c r="Z42" s="13"/>
       <c r="AA42" s="13"/>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>213</v>
       </c>
@@ -3596,7 +3765,7 @@
       <c r="Z43" s="13"/>
       <c r="AA43" s="13"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>1</v>
       </c>
@@ -3630,7 +3799,7 @@
       <c r="Z44" s="13"/>
       <c r="AA44" s="13"/>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>214</v>
       </c>
@@ -3667,7 +3836,7 @@
       <c r="Z45" s="13"/>
       <c r="AA45" s="13"/>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>4</v>
       </c>
@@ -3701,7 +3870,7 @@
       <c r="Z46" s="13"/>
       <c r="AA46" s="13"/>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
         <v>3</v>
       </c>
@@ -3735,7 +3904,7 @@
       <c r="Z47" s="13"/>
       <c r="AA47" s="13"/>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>215</v>
       </c>
@@ -3772,7 +3941,7 @@
       <c r="Z48" s="13"/>
       <c r="AA48" s="13"/>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
         <v>4</v>
       </c>
@@ -3806,7 +3975,7 @@
       <c r="Z49" s="13"/>
       <c r="AA49" s="13"/>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
         <v>3</v>
       </c>
@@ -3840,7 +4009,7 @@
       <c r="Z50" s="13"/>
       <c r="AA50" s="13"/>
     </row>
-    <row r="51" spans="1:27" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:27" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>208</v>
       </c>
@@ -3875,7 +4044,7 @@
       <c r="Z51" s="24"/>
       <c r="AA51" s="24"/>
     </row>
-    <row r="52" spans="1:27" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:27" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="23" t="s">
         <v>191</v>
       </c>
@@ -3909,7 +4078,7 @@
       <c r="Z52" s="24"/>
       <c r="AA52" s="24"/>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -3936,7 +4105,7 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -3963,7 +4132,7 @@
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -3990,7 +4159,7 @@
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -4017,7 +4186,7 @@
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -4044,7 +4213,7 @@
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -4076,4 +4245,594 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{488F58E0-11A9-4DD4-BEA4-AFCB0DF15156}">
+  <dimension ref="A1:AM11"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="22" width="13.7109375" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="39" width="9.28515625" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="U1" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+    </row>
+    <row r="2" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="B2" s="30">
+        <v>32</v>
+      </c>
+      <c r="C2" s="33">
+        <v>60</v>
+      </c>
+      <c r="D2" s="30">
+        <v>28</v>
+      </c>
+      <c r="E2" s="30">
+        <v>46</v>
+      </c>
+      <c r="F2" s="30">
+        <v>45</v>
+      </c>
+      <c r="G2" s="30">
+        <v>18</v>
+      </c>
+      <c r="H2" s="30">
+        <v>18</v>
+      </c>
+      <c r="I2" s="33">
+        <v>37</v>
+      </c>
+      <c r="J2" s="30">
+        <v>79</v>
+      </c>
+      <c r="K2" s="30">
+        <v>15</v>
+      </c>
+      <c r="L2" s="30">
+        <v>11</v>
+      </c>
+      <c r="M2" s="30">
+        <v>88</v>
+      </c>
+      <c r="N2" s="30">
+        <v>14</v>
+      </c>
+      <c r="O2" s="30">
+        <v>31</v>
+      </c>
+      <c r="P2" s="30">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="30">
+        <v>26</v>
+      </c>
+      <c r="R2" s="30">
+        <v>74</v>
+      </c>
+      <c r="S2" s="30">
+        <v>27</v>
+      </c>
+      <c r="T2" s="30">
+        <v>138</v>
+      </c>
+      <c r="U2" s="30">
+        <v>29</v>
+      </c>
+      <c r="V2" s="38">
+        <v>42</v>
+      </c>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+    </row>
+    <row r="3" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="30">
+        <v>15</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="N3" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="O3" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="P3" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q3" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="R3" s="30" t="s">
+        <v>297</v>
+      </c>
+      <c r="S3" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="T3" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="U3" s="30" t="s">
+        <v>300</v>
+      </c>
+      <c r="V3" s="38" t="s">
+        <v>301</v>
+      </c>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37"/>
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37"/>
+      <c r="AM3" s="37"/>
+    </row>
+    <row r="4" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="P4" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="37"/>
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="37"/>
+      <c r="AJ4" s="37"/>
+      <c r="AK4" s="37"/>
+      <c r="AL4" s="37"/>
+      <c r="AM4" s="37"/>
+    </row>
+    <row r="5" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="31">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="25">
+        <v>2.0950000000000002</v>
+      </c>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="25">
+        <v>2.08</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="25">
+        <v>1.913</v>
+      </c>
+      <c r="J5" s="25">
+        <v>1.97</v>
+      </c>
+      <c r="K5" s="25">
+        <v>1.89</v>
+      </c>
+      <c r="L5" s="25">
+        <v>1.91</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="N5" s="25">
+        <v>1.92</v>
+      </c>
+      <c r="O5" s="25">
+        <v>2.16</v>
+      </c>
+      <c r="P5" s="25">
+        <v>1.8</v>
+      </c>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="25">
+        <v>1.95</v>
+      </c>
+      <c r="V5" s="27"/>
+      <c r="W5" s="37">
+        <f>((B5*B2)+(D5*D2)+(G5*G2)+(I5*I2)+(J5*J2)+(K5*K2)+(L5*L2)+(N5*N2)+(O5*O2)+(P5*P2)+(U5*U2))/(B2+D2+G2+I2+J2+K2+L2+N2+O2+P2+U2)</f>
+        <v>1.9863089171974524</v>
+      </c>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="37"/>
+      <c r="AA5" s="37"/>
+      <c r="AB5" s="37"/>
+      <c r="AC5" s="37"/>
+      <c r="AD5" s="37"/>
+      <c r="AE5" s="37"/>
+      <c r="AF5" s="37"/>
+      <c r="AG5" s="37"/>
+      <c r="AH5" s="37"/>
+      <c r="AI5" s="37"/>
+      <c r="AJ5" s="37"/>
+      <c r="AK5" s="37"/>
+      <c r="AL5" s="37"/>
+      <c r="AM5" s="37"/>
+    </row>
+    <row r="6" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="W6" s="37"/>
+      <c r="X6" s="37"/>
+      <c r="Y6" s="37"/>
+      <c r="Z6" s="37"/>
+      <c r="AA6" s="37"/>
+      <c r="AB6" s="37"/>
+      <c r="AC6" s="37"/>
+      <c r="AD6" s="37"/>
+      <c r="AE6" s="37"/>
+      <c r="AF6" s="37"/>
+      <c r="AG6" s="37"/>
+      <c r="AH6" s="37"/>
+      <c r="AI6" s="37"/>
+      <c r="AJ6" s="37"/>
+      <c r="AK6" s="37"/>
+      <c r="AL6" s="37"/>
+      <c r="AM6" s="37"/>
+    </row>
+    <row r="7" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="31">
+        <v>4.8250000000000002</v>
+      </c>
+      <c r="C7" s="25">
+        <v>4.5</v>
+      </c>
+      <c r="D7" s="25">
+        <v>4.9550000000000001</v>
+      </c>
+      <c r="E7" s="25">
+        <v>4.29</v>
+      </c>
+      <c r="F7" s="25">
+        <v>3.67</v>
+      </c>
+      <c r="G7" s="25">
+        <v>5.03</v>
+      </c>
+      <c r="H7" s="25">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="I7" s="25">
+        <v>4.6470000000000002</v>
+      </c>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="25">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="M7" s="28">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="N7" s="25">
+        <v>4.49</v>
+      </c>
+      <c r="O7" s="27"/>
+      <c r="P7" s="25">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="25">
+        <v>5.05</v>
+      </c>
+      <c r="S7" s="25">
+        <v>4.4260000000000002</v>
+      </c>
+      <c r="T7" s="25">
+        <v>4.8</v>
+      </c>
+      <c r="U7" s="25">
+        <v>4.55</v>
+      </c>
+      <c r="V7" s="27"/>
+      <c r="W7" s="37">
+        <f>((B7*B2)+(C7*C2)+(D7*D2)+(E7*E2)+(F7*F2)+(G7*G2)+(H7*H2)+(I7*I2)+(L7*L2)+(M7*M2)+(N7*N2)+(P7*P2)+(R7*R2)+(S7*S2)+(T7*T2)+(U7*U2))/(B2+C2+D2+E2+F2+G2+H2+I2+L2+M2+N2+P2+R2+S2+T2+U2)</f>
+        <v>4.6430963503649627</v>
+      </c>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="37"/>
+      <c r="Z7" s="37"/>
+      <c r="AA7" s="37"/>
+      <c r="AB7" s="37"/>
+      <c r="AC7" s="37"/>
+      <c r="AD7" s="37"/>
+      <c r="AE7" s="37"/>
+      <c r="AF7" s="37"/>
+      <c r="AG7" s="37"/>
+      <c r="AH7" s="37"/>
+      <c r="AI7" s="37"/>
+      <c r="AJ7" s="37"/>
+      <c r="AK7" s="37"/>
+      <c r="AL7" s="37"/>
+      <c r="AM7" s="37"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="C11" s="40"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADAB502-DC3F-4544-AC59-7F12867491CB}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="28"/>
+      <c r="B1" s="28" t="s">
+        <v>347</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>350</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[note]: teorie hotova snad
</commit_message>
<xml_diff>
--- a/bc - tabulka výsledky.xlsx
+++ b/bc - tabulka výsledky.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7275a55917014348/Desktop/bakalarka/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1713" documentId="8_{BE3E68FC-0BCD-49A6-9D79-EB778FD7412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0759D99-FAB2-4D22-ADE1-F97F841E0502}"/>
+  <xr:revisionPtr revIDLastSave="1728" documentId="8_{BE3E68FC-0BCD-49A6-9D79-EB778FD7412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{951052AE-5CB5-40EF-9478-FB2E5337DCD3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{EC50F4EA-C447-47CC-B6F2-DF478986B29A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EC50F4EA-C447-47CC-B6F2-DF478986B29A}"/>
   </bookViews>
   <sheets>
     <sheet name="TABULKA" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="List2" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,6 +35,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1381,7 +1402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1489,13 +1510,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1824,15 +1841,15 @@
       <selection pane="bottomRight" sqref="A1:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" style="6" customWidth="1"/>
-    <col min="3" max="27" width="13.7109375" style="6" customWidth="1"/>
-    <col min="28" max="16384" width="9.28515625" style="6"/>
+    <col min="1" max="1" width="31.44140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" style="6" customWidth="1"/>
+    <col min="3" max="27" width="13.6640625" style="6" customWidth="1"/>
+    <col min="28" max="16384" width="9.33203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
@@ -1912,7 +1929,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>44</v>
       </c>
@@ -1992,7 +2009,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
@@ -2072,7 +2089,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>101</v>
       </c>
@@ -2125,7 +2142,7 @@
       <c r="Z4" s="7"/>
       <c r="AA4" s="14"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
@@ -2177,7 +2194,7 @@
       <c r="Z5" s="13"/>
       <c r="AA5" s="11"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
@@ -2227,7 +2244,7 @@
       </c>
       <c r="AA6" s="11"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
@@ -2289,7 +2306,7 @@
       <c r="Z7" s="13"/>
       <c r="AA7" s="11"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>269</v>
       </c>
@@ -2336,7 +2353,7 @@
       <c r="Z8" s="13"/>
       <c r="AA8" s="13"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -2377,7 +2394,7 @@
       <c r="Z9" s="13"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>152</v>
       </c>
@@ -2414,7 +2431,7 @@
       <c r="Z10" s="13"/>
       <c r="AA10" s="13"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
@@ -2471,7 +2488,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -2535,7 +2552,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
@@ -2579,7 +2596,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>277</v>
       </c>
@@ -2613,7 +2630,7 @@
       </c>
       <c r="AA14" s="13"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
@@ -2664,7 +2681,7 @@
       <c r="Z15" s="13"/>
       <c r="AA15" s="13"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -2708,7 +2725,7 @@
       <c r="Z16" s="13"/>
       <c r="AA16" s="13"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>273</v>
       </c>
@@ -2742,7 +2759,7 @@
       </c>
       <c r="AA17" s="13"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>274</v>
       </c>
@@ -2776,7 +2793,7 @@
       </c>
       <c r="AA18" s="13"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>275</v>
       </c>
@@ -2813,7 +2830,7 @@
       </c>
       <c r="AA19" s="13"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
@@ -2856,7 +2873,7 @@
       <c r="Z20" s="13"/>
       <c r="AA20" s="13"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
         <v>172</v>
       </c>
@@ -2888,7 +2905,7 @@
       <c r="Z21" s="13"/>
       <c r="AA21" s="13"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>170</v>
       </c>
@@ -2922,7 +2939,7 @@
       <c r="Z22" s="13"/>
       <c r="AA22" s="13"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>110</v>
       </c>
@@ -2957,7 +2974,7 @@
       <c r="Z23" s="13"/>
       <c r="AA23" s="13"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>111</v>
       </c>
@@ -2993,7 +3010,7 @@
       <c r="Z24" s="13"/>
       <c r="AA24" s="13"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>99</v>
       </c>
@@ -3042,7 +3059,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
         <v>97</v>
       </c>
@@ -3088,7 +3105,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>188</v>
       </c>
@@ -3125,7 +3142,7 @@
       <c r="Z27" s="13"/>
       <c r="AA27" s="13"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>189</v>
       </c>
@@ -3162,7 +3179,7 @@
       <c r="Z28" s="13"/>
       <c r="AA28" s="13"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>135</v>
       </c>
@@ -3197,7 +3214,7 @@
       <c r="Z29" s="13"/>
       <c r="AA29" s="13"/>
     </row>
-    <row r="30" spans="1:27" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>341</v>
       </c>
@@ -3254,7 +3271,7 @@
       <c r="Z30" s="13"/>
       <c r="AA30" s="13"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
         <v>342</v>
       </c>
@@ -3292,7 +3309,7 @@
       <c r="Z31" s="13"/>
       <c r="AA31" s="13"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
         <v>216</v>
       </c>
@@ -3328,7 +3345,7 @@
       <c r="Z32" s="13"/>
       <c r="AA32" s="13"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>8</v>
       </c>
@@ -3367,7 +3384,7 @@
       <c r="Z33" s="13"/>
       <c r="AA33" s="13"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
         <v>270</v>
       </c>
@@ -3403,7 +3420,7 @@
       <c r="Z34" s="13"/>
       <c r="AA34" s="13"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
         <v>6</v>
       </c>
@@ -3439,7 +3456,7 @@
       <c r="Z35" s="13"/>
       <c r="AA35" s="13"/>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>151</v>
       </c>
@@ -3484,7 +3501,7 @@
       <c r="Z36" s="13"/>
       <c r="AA36" s="13"/>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>98</v>
       </c>
@@ -3527,7 +3544,7 @@
       <c r="Z37" s="13"/>
       <c r="AA37" s="13"/>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>212</v>
       </c>
@@ -3582,7 +3599,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B39" s="6" t="s">
         <v>211</v>
       </c>
@@ -3614,7 +3631,7 @@
       <c r="Z39" s="13"/>
       <c r="AA39" s="13"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">
         <v>209</v>
       </c>
@@ -3650,7 +3667,7 @@
       <c r="Z40" s="13"/>
       <c r="AA40" s="13"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>150</v>
       </c>
@@ -3689,7 +3706,7 @@
       <c r="Z41" s="13"/>
       <c r="AA41" s="13"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>153</v>
       </c>
@@ -3728,7 +3745,7 @@
       <c r="Z42" s="13"/>
       <c r="AA42" s="13"/>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>213</v>
       </c>
@@ -3765,7 +3782,7 @@
       <c r="Z43" s="13"/>
       <c r="AA43" s="13"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B44" s="6" t="s">
         <v>1</v>
       </c>
@@ -3799,7 +3816,7 @@
       <c r="Z44" s="13"/>
       <c r="AA44" s="13"/>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>214</v>
       </c>
@@ -3836,7 +3853,7 @@
       <c r="Z45" s="13"/>
       <c r="AA45" s="13"/>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B46" s="6" t="s">
         <v>4</v>
       </c>
@@ -3870,7 +3887,7 @@
       <c r="Z46" s="13"/>
       <c r="AA46" s="13"/>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B47" s="6" t="s">
         <v>3</v>
       </c>
@@ -3904,7 +3921,7 @@
       <c r="Z47" s="13"/>
       <c r="AA47" s="13"/>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>215</v>
       </c>
@@ -3941,7 +3958,7 @@
       <c r="Z48" s="13"/>
       <c r="AA48" s="13"/>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B49" s="6" t="s">
         <v>4</v>
       </c>
@@ -3975,7 +3992,7 @@
       <c r="Z49" s="13"/>
       <c r="AA49" s="13"/>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B50" s="6" t="s">
         <v>3</v>
       </c>
@@ -4009,7 +4026,7 @@
       <c r="Z50" s="13"/>
       <c r="AA50" s="13"/>
     </row>
-    <row r="51" spans="1:27" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="23" t="s">
         <v>208</v>
       </c>
@@ -4044,7 +4061,7 @@
       <c r="Z51" s="24"/>
       <c r="AA51" s="24"/>
     </row>
-    <row r="52" spans="1:27" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="23" t="s">
         <v>191</v>
       </c>
@@ -4078,7 +4095,7 @@
       <c r="Z52" s="24"/>
       <c r="AA52" s="24"/>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -4105,7 +4122,7 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -4132,7 +4149,7 @@
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -4159,7 +4176,7 @@
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -4186,7 +4203,7 @@
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -4213,7 +4230,7 @@
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -4249,21 +4266,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{488F58E0-11A9-4DD4-BEA4-AFCB0DF15156}">
-  <dimension ref="A1:AM11"/>
+  <dimension ref="A1:AM32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="22" width="13.7109375" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="39" width="9.28515625" style="39"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="22" width="13.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
         <v>346</v>
       </c>
@@ -4330,25 +4346,25 @@
       <c r="V1" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-    </row>
-    <row r="2" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="6"/>
+    </row>
+    <row r="2" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="34" t="s">
         <v>345</v>
       </c>
@@ -4412,28 +4428,28 @@
       <c r="U2" s="30">
         <v>29</v>
       </c>
-      <c r="V2" s="38">
+      <c r="V2" s="37">
         <v>42</v>
       </c>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="37"/>
-    </row>
-    <row r="3" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
+      <c r="AM2" s="6"/>
+    </row>
+    <row r="3" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>344</v>
       </c>
@@ -4497,28 +4513,28 @@
       <c r="U3" s="30" t="s">
         <v>300</v>
       </c>
-      <c r="V3" s="38" t="s">
+      <c r="V3" s="37" t="s">
         <v>301</v>
       </c>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
-      <c r="AK3" s="37"/>
-      <c r="AL3" s="37"/>
-      <c r="AM3" s="37"/>
-    </row>
-    <row r="4" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" s="6"/>
+      <c r="AM3" s="6"/>
+    </row>
+    <row r="4" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
         <v>21</v>
       </c>
@@ -4563,25 +4579,25 @@
       <c r="T4" s="32"/>
       <c r="U4" s="32"/>
       <c r="V4" s="32"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="37"/>
-      <c r="AA4" s="37"/>
-      <c r="AB4" s="37"/>
-      <c r="AC4" s="37"/>
-      <c r="AD4" s="37"/>
-      <c r="AE4" s="37"/>
-      <c r="AF4" s="37"/>
-      <c r="AG4" s="37"/>
-      <c r="AH4" s="37"/>
-      <c r="AI4" s="37"/>
-      <c r="AJ4" s="37"/>
-      <c r="AK4" s="37"/>
-      <c r="AL4" s="37"/>
-      <c r="AM4" s="37"/>
-    </row>
-    <row r="5" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+    </row>
+    <row r="5" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
         <v>20</v>
       </c>
@@ -4628,28 +4644,28 @@
         <v>1.95</v>
       </c>
       <c r="V5" s="27"/>
-      <c r="W5" s="37">
+      <c r="W5" s="6">
         <f>((B5*B2)+(D5*D2)+(G5*G2)+(I5*I2)+(J5*J2)+(K5*K2)+(L5*L2)+(N5*N2)+(O5*O2)+(P5*P2)+(U5*U2))/(B2+D2+G2+I2+J2+K2+L2+N2+O2+P2+U2)</f>
         <v>1.9863089171974524</v>
       </c>
-      <c r="X5" s="37"/>
-      <c r="Y5" s="37"/>
-      <c r="Z5" s="37"/>
-      <c r="AA5" s="37"/>
-      <c r="AB5" s="37"/>
-      <c r="AC5" s="37"/>
-      <c r="AD5" s="37"/>
-      <c r="AE5" s="37"/>
-      <c r="AF5" s="37"/>
-      <c r="AG5" s="37"/>
-      <c r="AH5" s="37"/>
-      <c r="AI5" s="37"/>
-      <c r="AJ5" s="37"/>
-      <c r="AK5" s="37"/>
-      <c r="AL5" s="37"/>
-      <c r="AM5" s="37"/>
-    </row>
-    <row r="6" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
+      <c r="AM5" s="6"/>
+    </row>
+    <row r="6" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="34" t="s">
         <v>19</v>
       </c>
@@ -4694,25 +4710,25 @@
       <c r="V6" s="25" t="s">
         <v>306</v>
       </c>
-      <c r="W6" s="37"/>
-      <c r="X6" s="37"/>
-      <c r="Y6" s="37"/>
-      <c r="Z6" s="37"/>
-      <c r="AA6" s="37"/>
-      <c r="AB6" s="37"/>
-      <c r="AC6" s="37"/>
-      <c r="AD6" s="37"/>
-      <c r="AE6" s="37"/>
-      <c r="AF6" s="37"/>
-      <c r="AG6" s="37"/>
-      <c r="AH6" s="37"/>
-      <c r="AI6" s="37"/>
-      <c r="AJ6" s="37"/>
-      <c r="AK6" s="37"/>
-      <c r="AL6" s="37"/>
-      <c r="AM6" s="37"/>
-    </row>
-    <row r="7" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="6"/>
+      <c r="AM6" s="6"/>
+    </row>
+    <row r="7" spans="1:39" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="34" t="s">
         <v>18</v>
       </c>
@@ -4769,29 +4785,533 @@
         <v>4.55</v>
       </c>
       <c r="V7" s="27"/>
-      <c r="W7" s="37">
+      <c r="W7" s="6">
         <f>((B7*B2)+(C7*C2)+(D7*D2)+(E7*E2)+(F7*F2)+(G7*G2)+(H7*H2)+(I7*I2)+(L7*L2)+(M7*M2)+(N7*N2)+(P7*P2)+(R7*R2)+(S7*S2)+(T7*T2)+(U7*U2))/(B2+C2+D2+E2+F2+G2+H2+I2+L2+M2+N2+P2+R2+S2+T2+U2)</f>
         <v>4.6430963503649627</v>
       </c>
-      <c r="X7" s="37"/>
-      <c r="Y7" s="37"/>
-      <c r="Z7" s="37"/>
-      <c r="AA7" s="37"/>
-      <c r="AB7" s="37"/>
-      <c r="AC7" s="37"/>
-      <c r="AD7" s="37"/>
-      <c r="AE7" s="37"/>
-      <c r="AF7" s="37"/>
-      <c r="AG7" s="37"/>
-      <c r="AH7" s="37"/>
-      <c r="AI7" s="37"/>
-      <c r="AJ7" s="37"/>
-      <c r="AK7" s="37"/>
-      <c r="AL7" s="37"/>
-      <c r="AM7" s="37"/>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C11" s="40"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A11" t="str" cm="1">
+        <f t="array" ref="A11:G32">TRANSPOSE(A1:V7)</f>
+        <v>Studie</v>
+      </c>
+      <c r="B11" t="str">
+        <v xml:space="preserve">⌀ počet účastníků </v>
+      </c>
+      <c r="C11" s="38" t="str">
+        <v xml:space="preserve">⌀ věk </v>
+      </c>
+      <c r="D11" t="str">
+        <v>⌀ čas na 5 m (s)</v>
+      </c>
+      <c r="E11" t="str">
+        <v>⌀ čas na 10 m (s)</v>
+      </c>
+      <c r="F11" t="str">
+        <v>⌀ čas na 20 m (s)</v>
+      </c>
+      <c r="G11" t="str">
+        <v>⌀ čas na 30 m (s)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <v>Studie 1</v>
+      </c>
+      <c r="B12">
+        <v>32</v>
+      </c>
+      <c r="C12" t="str">
+        <v>16,6 ± 0,6</v>
+      </c>
+      <c r="D12" t="str">
+        <v>1,175 ± 0,051</v>
+      </c>
+      <c r="E12">
+        <v>2.0449999999999999</v>
+      </c>
+      <c r="F12" t="str">
+        <v>3,549 ± 0,212</v>
+      </c>
+      <c r="G12">
+        <v>4.8250000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <v>Studie 2</v>
+      </c>
+      <c r="B13">
+        <v>60</v>
+      </c>
+      <c r="C13" t="str">
+        <v>15-15,9</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <v>Studie 3</v>
+      </c>
+      <c r="B14">
+        <v>28</v>
+      </c>
+      <c r="C14" t="str">
+        <v>14,55 ± 0,25</v>
+      </c>
+      <c r="D14" t="str">
+        <v>1,21 ± 0,05</v>
+      </c>
+      <c r="E14">
+        <v>2.0950000000000002</v>
+      </c>
+      <c r="F14" t="str">
+        <v>3,62 ± 0,215</v>
+      </c>
+      <c r="G14">
+        <v>4.9550000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <v>Studie 4</v>
+      </c>
+      <c r="B15">
+        <v>46</v>
+      </c>
+      <c r="C15" t="str">
+        <v>14,83 ± 0,64</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <v>Studie 6</v>
+      </c>
+      <c r="B16">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="str">
+        <v>1,22 ± 0,15</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>3.67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <v>Studie 7</v>
+      </c>
+      <c r="B17">
+        <v>18</v>
+      </c>
+      <c r="C17" t="str">
+        <v>14,7 ± 0,3</v>
+      </c>
+      <c r="D17" t="str">
+        <v>1,21 ± 0,06</v>
+      </c>
+      <c r="E17">
+        <v>2.08</v>
+      </c>
+      <c r="F17" t="str">
+        <v>3,73 ± 0,19</v>
+      </c>
+      <c r="G17">
+        <v>5.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <v>Studie 8</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+      <c r="C18" t="str">
+        <v xml:space="preserve">15,1 ± 0,32	</v>
+      </c>
+      <c r="D18" t="str">
+        <v>1,06 ± 0,08</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>4.5199999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <v>Studie 9</v>
+      </c>
+      <c r="B19">
+        <v>37</v>
+      </c>
+      <c r="C19" t="str">
+        <v>14,7 ± 0,4</v>
+      </c>
+      <c r="D19" t="str">
+        <v xml:space="preserve"> 1,118 ± 0,054</v>
+      </c>
+      <c r="E19">
+        <v>1.913</v>
+      </c>
+      <c r="F19" t="str">
+        <v xml:space="preserve"> 3,306 ± 0,135</v>
+      </c>
+      <c r="G19">
+        <v>4.6470000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <v>Studie 10</v>
+      </c>
+      <c r="B20">
+        <v>79</v>
+      </c>
+      <c r="C20" t="str">
+        <v>14,5 ± 0,3</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1.97</v>
+      </c>
+      <c r="F20" t="str">
+        <v>3,40 ± 0,19</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <v>Studie 11</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21" t="str">
+        <v>14,4 ± 0,5</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1.89</v>
+      </c>
+      <c r="F21" t="str">
+        <v>3,25 ± 0,11</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <v>Studie 12</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22" t="str">
+        <v>14,9 ± 0,7</v>
+      </c>
+      <c r="D22" t="str">
+        <v>1,12 ± 0,04</v>
+      </c>
+      <c r="E22">
+        <v>1.91</v>
+      </c>
+      <c r="F22" t="str">
+        <v>3,28 ± 0,10</v>
+      </c>
+      <c r="G22">
+        <v>4.5599999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <v>Studie 13</v>
+      </c>
+      <c r="B23">
+        <v>88</v>
+      </c>
+      <c r="C23" t="str">
+        <v>14,05 ± 0,35</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <v>Studie 15</v>
+      </c>
+      <c r="B24">
+        <v>14</v>
+      </c>
+      <c r="C24" t="str">
+        <v>15-15,9</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1.92</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <v>Studie 16</v>
+      </c>
+      <c r="B25">
+        <v>31</v>
+      </c>
+      <c r="C25" t="str">
+        <v>16,36  ± 0,5</v>
+      </c>
+      <c r="D25" t="str">
+        <v>1,22 ± 0,07</v>
+      </c>
+      <c r="E25">
+        <v>2.16</v>
+      </c>
+      <c r="F25" t="str">
+        <v>3,57 ± 0,22</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <v>Studie 17</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="C26" t="str">
+        <v>15-15,9</v>
+      </c>
+      <c r="D26" t="str">
+        <v>1,04 ± 0,05</v>
+      </c>
+      <c r="E26">
+        <v>1.8</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <v>Studie 18</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="str">
+        <v>16,2 ± 0,9</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="str">
+        <v>3,13 ± 0,25</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <v>Studie 19</v>
+      </c>
+      <c r="B28">
+        <v>74</v>
+      </c>
+      <c r="C28" t="str">
+        <v>14,11 ± 0,58</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <v>Studie 20</v>
+      </c>
+      <c r="B29">
+        <v>27</v>
+      </c>
+      <c r="C29" t="str">
+        <v xml:space="preserve"> 16,408 ± 0,843</v>
+      </c>
+      <c r="D29" t="str">
+        <v>1,094 ± 0,074</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>4.4260000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <v>Studie 22</v>
+      </c>
+      <c r="B30">
+        <v>138</v>
+      </c>
+      <c r="C30" t="str">
+        <v>14,1 ± 0,5</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <v>Studie 23</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="C31" t="str">
+        <v>16,5 ± 0,8</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1.95</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <v>Studie 24</v>
+      </c>
+      <c r="B32">
+        <v>42</v>
+      </c>
+      <c r="C32" t="str">
+        <v>16,0 ± 1,3</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="str">
+        <v xml:space="preserve">3,1 ± 0,3 </v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4803,13 +5323,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADAB502-DC3F-4544-AC59-7F12867491CB}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="28"/>
       <c r="B1" s="28" t="s">
         <v>347</v>
@@ -4818,14 +5338,14 @@
         <v>348</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>349</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>350</v>
       </c>

</xml_diff>